<commit_message>
Adding codes and files, modify the index and add principle.
</commit_message>
<xml_diff>
--- a/bootstrap_lib.xlsx
+++ b/bootstrap_lib.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="13395" windowHeight="9525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t xml:space="preserve">&lt;!DOCTYPE html&gt;
 &lt;html&gt;
@@ -791,21 +791,44 @@
   &lt;/div&gt;
 &lt;/div&gt;</t>
   </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Code Ref</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="2"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -815,6 +838,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -831,24 +860,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -922,6 +962,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -956,6 +997,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1131,490 +1173,502 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="39" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="81.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39" customHeight="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39" customHeight="1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="39" customHeight="1">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="39" customHeight="1">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="39" customHeight="1">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="39" customHeight="1">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="39" customHeight="1">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="39" customHeight="1">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="39" customHeight="1">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="39" customHeight="1">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="39" customHeight="1">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="39" customHeight="1">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="39" customHeight="1">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="39" customHeight="1">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="39" customHeight="1">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="39" customHeight="1">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="39" customHeight="1">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="39" customHeight="1">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="39" customHeight="1">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="39" customHeight="1">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="39" customHeight="1">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="39" customHeight="1">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="39" customHeight="1">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="39" customHeight="1">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="39" customHeight="1">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="39" customHeight="1">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="39" customHeight="1">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="39" customHeight="1">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    <row r="29" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="39" customHeight="1">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="30" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="39" customHeight="1">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3" t="s">
+    <row r="31" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="39" customHeight="1">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3" t="s">
+    <row r="32" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="39" customHeight="1">
-      <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="3" t="s">
+    <row r="33" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="39" customHeight="1">
-      <c r="A33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3" t="s">
+    <row r="34" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="39" customHeight="1">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="3" t="s">
+    <row r="35" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="39" customHeight="1">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="3" t="s">
+    <row r="36" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="39" customHeight="1">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="3" t="s">
+    <row r="37" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="39" customHeight="1">
-      <c r="A37" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="38" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="39" customHeight="1">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
+    <row r="39" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="39" customHeight="1">
-      <c r="A39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
+    <row r="40" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="39" customHeight="1">
-      <c r="A40" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="39" customHeight="1">
+    <row r="41" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="39" customHeight="1">
+    <row r="42" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="43" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>